<commit_message>
Update firmware, building instructions.
</commit_message>
<xml_diff>
--- a/Models/WIFI_Car/WiFi-Car-BOM.xlsx
+++ b/Models/WIFI_Car/WiFi-Car-BOM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="615" windowWidth="27495" windowHeight="12210"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -226,8 +231,545 @@
 </sst>
 </file>
 
+<file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="18" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+  </fonts>
+  <fills count="33">
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+  </fills>
+  <borders count="10">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+  </borders>
+  <cellStyleXfs count="42">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </cellXfs>
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
+</styleSheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -249,23 +791,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="1038225"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -293,23 +835,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="1876425"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -337,23 +879,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="2714625"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -381,23 +923,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="3552825"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -425,23 +967,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image5">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="4391025"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -469,23 +1011,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image6">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="5229225"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -513,23 +1055,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image7">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="6067425"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -557,23 +1099,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image8">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="6905625"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -601,23 +1143,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image9">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="7743825"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -645,23 +1187,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image10">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="8582025"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -689,23 +1231,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image11">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="9420225"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -733,23 +1275,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image12">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="10258425"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -777,23 +1319,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image13">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="11096625"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -821,23 +1363,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image14">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="11934825"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -865,23 +1407,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image15">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="12773025"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -909,23 +1451,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image16">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="13611225"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -953,23 +1495,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image17">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="14449425"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -997,23 +1539,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image18">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="15287625"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1041,23 +1583,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image19">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="16125825"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1085,23 +1627,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image20">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="16964025"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1129,23 +1671,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image21">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="17802225"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1173,23 +1715,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image22">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="18640425"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1217,23 +1759,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image23">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="19478625"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1261,23 +1803,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image24">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="20316825"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1305,23 +1847,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image25">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="21155025"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1349,23 +1891,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image26">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="21993225"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1393,23 +1935,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image27">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="22831425"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1437,23 +1979,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image28">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="23669625"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1481,23 +2023,23 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image29">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:xfrm>
           <a:off x="3448050" y="24507825"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -1507,21 +2049,307 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32" bestFit="1"/>
     <col min="5" max="5" width="25" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1541,7 +2369,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="66" customHeight="1">
+    <row r="2" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1558,7 +2386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="66" customHeight="1">
+    <row r="3" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +2403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="66" customHeight="1">
+    <row r="4" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1592,7 +2420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="66" customHeight="1">
+    <row r="5" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1609,7 +2437,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="66" customHeight="1">
+    <row r="6" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1626,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="66" customHeight="1">
+    <row r="7" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1643,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="66" customHeight="1">
+    <row r="8" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1660,7 +2488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="66" customHeight="1">
+    <row r="9" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1677,7 +2505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="66" customHeight="1">
+    <row r="10" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1694,7 +2522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="66" customHeight="1">
+    <row r="11" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1711,7 +2539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="66" customHeight="1">
+    <row r="12" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1728,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="66" customHeight="1">
+    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1745,7 +2573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="66" customHeight="1">
+    <row r="14" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1762,7 +2590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="66" customHeight="1">
+    <row r="15" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1779,7 +2607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="66" customHeight="1">
+    <row r="16" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1796,7 +2624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="66" customHeight="1">
+    <row r="17" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1813,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="66" customHeight="1">
+    <row r="18" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1830,7 +2658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="66" customHeight="1">
+    <row r="19" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1847,7 +2675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="66" customHeight="1">
+    <row r="20" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -1864,7 +2692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="66" customHeight="1">
+    <row r="21" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1881,7 +2709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="66" customHeight="1">
+    <row r="22" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1898,7 +2726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="66" customHeight="1">
+    <row r="23" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1915,7 +2743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="66" customHeight="1">
+    <row r="24" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1932,7 +2760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="66" customHeight="1">
+    <row r="25" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>58</v>
       </c>
@@ -1949,7 +2777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="66" customHeight="1">
+    <row r="26" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>60</v>
       </c>
@@ -1966,7 +2794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="66" customHeight="1">
+    <row r="27" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1983,7 +2811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="66" customHeight="1">
+    <row r="28" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -2000,7 +2828,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="66" customHeight="1">
+    <row r="29" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -2017,7 +2845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="66" customHeight="1">
+    <row r="30" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -2034,15 +2862,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>70</v>
       </c>
       <c r="F31">
         <f>SUM(F2:F30)</f>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>